<commit_message>
basic data transfer correct
</commit_message>
<xml_diff>
--- a/jobs_data.xlsx
+++ b/jobs_data.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,48 +434,443 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Vývojář/Analytik Databáze/SQL</t>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>job_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>company_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>address_street</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>address_city</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>address_district</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>responsible_name</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>first_number</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>second_number</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>matching_words</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>html_text</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Automation Developer</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ASB Czech Republic, s.r.o.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>V celnici 1031/4</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Praha</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Nové Město</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Pracovní nabídka
-Staňte se součástí logistické divize SEACOMP vyvíjející rozsáhlé robotizované logistické informační systémy. Podílíme se na implementaci a managementu produkčních systémů o velikosti až 120.000 m2 v rámci celého evropského prostoru.
-Předmětem Vaší práce bude:
-- Vývoj backendu logistického informačního systému – platforma PL/SQL
-- Návrh a implementace změn ve warehouse procesech s důrazem na zvyšování výkonnosti
-- Nasazení implementace do produkčního systému
-- Provádění integračních a akceptačních testů
-Požadujeme:
-- Práce na plný úvazek, přechodně možno i na částečný
-- Znalost programování relačních databází (ORACLE není podmínkou): SQL nebo některý ze strukturovaných jazyků (I-SQL, T-SQL, PL/SQL, …)
-- Aktivní přístup při řešení projektů
-- Vysokoškolské vzdělání technického směru
-- Zodpovědnost a smysl pro práci v týmu
-Nabízíme:
-- Nadstandardní platové ohodnocení – nechte si vypracovat individuální nabídku, talenty umíme ocenit
-- Pružná pracovní doba – máme řešení pro ranní ptáčata i večerní sovy
-- Přátelské a kolegiální pracovní prostředí ve zcela nové polyfunkční budově v naprostém centru Brna
-- Odborné školení, možnost seznámit se s širokým spektrem aktuálních vývojových technologií
-- Možnost krátkodobých služebních cest do zahraničí
-- Možnost využít firemní chill-out zónu přímo na pracovišti (fotbálek, ergonometr, rotoped, grill bar, aj.)
-- Penzijní připojištění, příspěvky na stravování, mobilní telefon, notebook
-- Široká škála mimofiremních aktivit (dračí lodě, cyklovýlety, lyžování, sportovní turnaje, …)
-Nástup je možný ihned nebo dle dohody.
-Pokud máte o tuto pozici zájem, pošlete prosím Váš strukturovaný životopis na e-mail jobs(a)seacomp.cz nebo nás kontaktuje telefonicky na tel. čísle + 420 608 736 650
-Velmi se těšíme se na spolupráci s Vámi.
-SEACOMP S.R.O., BRANDLOVA 4, 602 00 BRNO, DRŽITEL CERTIFIKACE ISO 9001:2015 ISO 14001:2015 ISO 27001:2013</t>
+ASB Group je profesionální outsourcingová společnost poskytující služby nadstandardní úrovně v oblasti zakládání společností, účetnictví, reportingu, daňového poradenství, trust managementu a mzdové agendy. Vznikla v roce 2002 a na pobočkách v Praze, Varšavě, Bratislavě, Budapešti a také Toruni zaměstnává přes 400 lidí. ASB Czech Republic s.r.o. právě rozšiřuje řady automatizačního týmu. Hledáme novou posilu s drivem a autentickým zájmem o automatizace, optimalizace, zlepšování procesů. Hledáme talentovaného nadšence, který se nebojí velkých výzev.
+Baví tě hledat způsoby jak dělat věci efektivněji? Jsi schopný/á vést s nadšením konverzaci o technologiích od rána do večera? Změnila ti ChatGPT aspoň trochu život?
+Nechceš si to v práci jen odsedět, ale investovat do toho něco sám/a za sebe? Už jsi někdy použil/a pozdrav „Hello, World!"? Hledáme juniorního kolegu do automatizačního týmu. Ve spolupráci s týmovým kolegou budeš mít stále dost velkou odpovědnost a tvoje rozhodnutí budou udávat dlouhodobý směr automatizace v naší firmě. Zároveň ale budeš mít vždy na koho se obrátit a kdo tě v případě potřeby povede.
+Co budeme potřebovat:
+Analytické myšlení a proaktivní přístup
+Dobrou spolupráci jak remote, tak v kanceláři
+SELECT * FROM zaklady_SQL;
+Pokročilou znalost Excelu
+Aktivní komunikaci v AJ alespoň na úrovni B1
+Schopnost naučit se nové technologie (jazyk, platforma, ERP, AI nástroj)
+Bude super, když budeš mít:
+Mírně pokročilou znalost nějakého programovacího jazyka
+Zkušenost s aktivním používáním AI
+Jakékoliv zkušenosti s MS Power platformou, testováním aplikací, RPA nebo API
+Co budeš u nás dělat:
+Vytvářet jednoduché automatizační nástroje pro kolegy
+Podílet se na složitějších řešeních, které budou používat celá oddělení
+Spolupracovat a hledat možnosti jak může AI a jiné technologie ulehčit naši práci
+Udržovat, opravovat a vylepšovat stávající řešení
+Používat ChatGPT, Copiloty a Git na denní bázi
+Časem ovládat spoustu daňových a účetních výrazů 😊
+def a_hodne():
+try:
+print(testovat)
+except NameError:
+print("testovat!")
+S čím budeš pracovat:
+Naše současné řešení jsou ve VBA, Power Automate a Pythonu
+Pro robotizace používáme RPA Power Automate Desktop
+Prostředí - Windows
+Hodně pracujeme s Excelovskými tabulkami, XML soubory, účetním systémem Helios a databázemi
+Co ti nabídneme:
+Flexibilní pracovní dobu
+Velmi zajímavé platové ohodnocení
+Mladý dynamický kolektiv příjemné pracovní prostředí v centru Prahy
+Profesní růst a odborné vzdělávání
+Zajímavé platové ohodnocení + pravidelné bonusy
+Zaměstnanecké benefity (dovolená navíc, stravenkový paušál, systém cafeterie - individuální čerpání benefitů, jazykové a odborné vzdělávání, pravidelné teambuildingy)
+Flexibilní pracovní dobu, možnost práce z domova
+Občerstvení na pracovišti každý den</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Petra Hořejší</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>224 931 366</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>&lt;div&gt;&lt;p&gt;Pracovní nabídka&lt;/p&gt;&lt;p&gt;&lt;strong&gt;ASB Group je profesionální outsourcingová společnost poskytující služby nadstandardní úrovně v oblasti zakládání společností, účetnictví, reportingu, daňového poradenství, trust managementu a mzdové agendy. Vznikla v roce 2002 a na pobočkách v Praze, Varšavě, Bratislavě, Budapešti a také Toruni zaměstnává přes 400 lidí. ASB Czech Republic s.r.o. právě rozšiřuje řady automatizačního týmu. Hledáme novou posilu s drivem a autentickým zájmem o automatizace, optimalizace, zlepšování procesů. Hledáme talentovaného nadšence, který se nebojí velkých výzev.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Baví tě hledat způsoby jak dělat věci efektivněji? Jsi schopný/á vést s nadšením konverzaci o technologiích od rána do večera? Změnila ti ChatGPT aspoň trochu život?&lt;/p&gt;&lt;p&gt;Nechceš si to v práci jen odsedět, ale investovat do toho něco sám/a za sebe? Už jsi někdy použil/a pozdrav „Hello, World!"? Hledáme juniorního kolegu do automatizačního týmu. Ve spolupráci s týmovým kolegou budeš mít stále dost velkou odpovědnost a tvoje rozhodnutí budou udávat dlouhodobý směr automatizace v naší firmě. Zároveň ale budeš mít vždy na koho se obrátit a kdo tě v případě potřeby povede.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Co budeme potřebovat:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Analytické myšlení a proaktivní přístup&lt;/li&gt;&lt;li&gt;Dobrou spolupráci jak remote, tak v kanceláři&lt;/li&gt;&lt;li&gt;SELECT * FROM zaklady_SQL;&lt;/li&gt;&lt;li&gt;Pokročilou znalost Excelu&lt;/li&gt;&lt;li&gt;Aktivní komunikaci v AJ alespoň na úrovni B1&lt;/li&gt;&lt;li&gt;Schopnost naučit se nové technologie (jazyk, platforma, ERP, AI nástroj)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Bude super, když budeš mít:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Mírně pokročilou znalost nějakého programovacího jazyka&lt;/li&gt;&lt;li&gt;Zkušenost s aktivním používáním AI&lt;/li&gt;&lt;li&gt;Jakékoliv zkušenosti s MS Power platformou, testováním aplikací, RPA nebo API&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Co budeš u nás dělat:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Vytvářet jednoduché automatizační nástroje pro kolegy&lt;/li&gt;&lt;li&gt;Podílet se na složitějších řešeních, které budou používat celá oddělení&lt;/li&gt;&lt;li&gt;Spolupracovat a hledat možnosti jak může AI a jiné technologie ulehčit naši práci&lt;/li&gt;&lt;li&gt;Udržovat, opravovat a vylepšovat stávající řešení&lt;/li&gt;&lt;li&gt;Používat ChatGPT, Copiloty a Git na denní bázi&lt;/li&gt;&lt;li&gt;Časem ovládat spoustu daňových a účetních výrazů 😊&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;em&gt;def a_hodne():&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; try:&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; print(testovat)&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; except NameError:&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; print("testovat!")&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;S čím budeš pracovat:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Naše současné řešení jsou ve VBA, Power Automate a Pythonu&lt;/li&gt;&lt;li&gt;Pro robotizace používáme RPA Power Automate Desktop&lt;/li&gt;&lt;li&gt;Prostředí - Windows&lt;/li&gt;&lt;li&gt;Hodně pracujeme s Excelovskými tabulkami, XML soubory, účetním systémem Helios a databázemi&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Co ti nabídneme:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Flexibilní pracovní dobu&lt;/li&gt;&lt;li&gt;Velmi zajímavé platové ohodnocení&lt;/li&gt;&lt;li&gt;Mladý dynamický kolektiv příjemné pracovní prostředí v centru Prahy&lt;/li&gt;&lt;li&gt;Profesní růst a odborné vzdělávání&lt;/li&gt;&lt;li&gt;Zajímavé platové ohodnocení + pravidelné bonusy&lt;/li&gt;&lt;li&gt;Zaměstnanecké benefity (dovolená navíc, stravenkový paušál, systém cafeterie - individuální čerpání benefitů, jazykové a odborné vzdělávání, pravidelné teambuildingy)&lt;/li&gt;&lt;li&gt;Flexibilní pracovní dobu, možnost práce z domova&lt;/li&gt;&lt;li&gt;Občerstvení na pracovišti každý den&lt;/li&gt;&lt;/ul&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>&lt;div&gt;&lt;p&gt;Pracovní nabídka&lt;/p&gt;&lt;p&gt;Staňte se součástí logistické divize SEACOMP vyvíjející rozsáhlé robotizované logistické informační systémy. Podílíme se na implementaci a managementu produkčních systémů o velikosti až 120.000 m2 v rámci celého evropského prostoru. &lt;br&gt; &lt;br&gt;Předmětem Vaší práce bude: &lt;br&gt; &lt;br&gt;- Vývoj backendu logistického informačního systému – platforma PL/SQL &lt;br&gt;&lt;/br&gt;- Návrh a implementace změn ve warehouse procesech s důrazem na zvyšování výkonnosti&lt;br&gt;&lt;/br&gt;- Nasazení implementace do produkčního systému &lt;br&gt;&lt;/br&gt; - Provádění integračních a akceptačních testů&lt;br&gt;&lt;/br&gt;&lt;br&gt;&lt;/br&gt;Požadujeme: &lt;br&gt;&lt;/br&gt; &lt;br&gt;&lt;/br&gt;- Práce na plný úvazek, přechodně možno i na částečný &lt;br&gt;&lt;/br&gt;- Znalost programování relačních databází (ORACLE není podmínkou): SQL nebo některý ze strukturovaných jazyků (I-SQL, T-SQL, PL/SQL, …) &lt;br&gt;&lt;/br&gt;- Aktivní přístup při řešení projektů &lt;br&gt;&lt;/br&gt;- Vysokoškolské vzdělání technického směru &lt;br&gt;&lt;/br&gt;- Zodpovědnost a smysl pro práci v týmu &lt;br&gt;&lt;/br&gt; &lt;br&gt;&lt;/br&gt;Nabízíme:&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;&lt;/p&gt;&lt;p&gt;- Nadstandardní platové ohodnocení – nechte si vypracovat individuální nabídku, talenty umíme ocenit&lt;br&gt;&lt;/br&gt;- Pružná pracovní doba – máme řešení pro ranní ptáčata i večerní sovy&lt;br&gt;&lt;/br&gt;- Přátelské a kolegiální pracovní prostředí ve zcela nové polyfunkční budově v naprostém centru Brna&lt;br&gt;&lt;/br&gt;- Odborné školení, možnost seznámit se s širokým spektrem aktuálních vývojových technologií&lt;br&gt;&lt;/br&gt;- Možnost krátkodobých služebních cest do zahraničí&lt;br&gt;&lt;/br&gt;- Možnost využít firemní chill-out zónu přímo na pracovišti (fotbálek, ergonometr, rotoped, grill bar, aj.)&lt;br&gt;&lt;/br&gt;- Penzijní připojištění, příspěvky na stravování, mobilní telefon, notebook&lt;br&gt;&lt;/br&gt;- Široká škála mimofiremních aktivit (dračí lodě, cyklovýlety, lyžování, sportovní turnaje, …)&lt;/p&gt;&lt;p&gt;Nástup je možný ihned nebo dle dohody.&lt;/p&gt;&lt;p&gt;Pokud máte o tuto pozici zájem, pošlete prosím Váš strukturovaný životopis na e-mail jobs(a)seacomp.cz nebo nás kontaktuje telefonicky na tel. čísle + 420 608 736 650&lt;/p&gt;&lt;p&gt;Velmi se těšíme se na spolupráci s Vámi.&lt;/p&gt;&lt;p&gt;SEACOMP S.R.O., BRANDLOVA 4, 602 00 BRNO, DRŽITEL CERTIFIKACE ISO 9001:2015 ISO 14001:2015 ISO 27001:2013&lt;/p&gt;&lt;/div&gt;</t>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Automation Developer</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ASB Czech Republic, s.r.o.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>V celnici 1031/4</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Praha</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Nové Město</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Pracovní nabídka
+ASB Group je profesionální outsourcingová společnost poskytující služby nadstandardní úrovně v oblasti zakládání společností, účetnictví, reportingu, daňového poradenství, trust managementu a mzdové agendy. Vznikla v roce 2002 a na pobočkách v Praze, Varšavě, Bratislavě, Budapešti a také Toruni zaměstnává přes 400 lidí. ASB Czech Republic s.r.o. právě rozšiřuje řady automatizačního týmu. Hledáme novou posilu s drivem a autentickým zájmem o automatizace, optimalizace, zlepšování procesů. Hledáme talentovaného nadšence, který se nebojí velkých výzev.
+Baví tě hledat způsoby jak dělat věci efektivněji? Jsi schopný/á vést s nadšením konverzaci o technologiích od rána do večera? Změnila ti ChatGPT aspoň trochu život?
+Nechceš si to v práci jen odsedět, ale investovat do toho něco sám/a za sebe? Už jsi někdy použil/a pozdrav „Hello, World!"? Hledáme juniorního kolegu do automatizačního týmu. Ve spolupráci s týmovým kolegou budeš mít stále dost velkou odpovědnost a tvoje rozhodnutí budou udávat dlouhodobý směr automatizace v naší firmě. Zároveň ale budeš mít vždy na koho se obrátit a kdo tě v případě potřeby povede.
+Co budeme potřebovat:
+Analytické myšlení a proaktivní přístup
+Dobrou spolupráci jak remote, tak v kanceláři
+SELECT * FROM zaklady_SQL;
+Pokročilou znalost Excelu
+Aktivní komunikaci v AJ alespoň na úrovni B1
+Schopnost naučit se nové technologie (jazyk, platforma, ERP, AI nástroj)
+Bude super, když budeš mít:
+Mírně pokročilou znalost nějakého programovacího jazyka
+Zkušenost s aktivním používáním AI
+Jakékoliv zkušenosti s MS Power platformou, testováním aplikací, RPA nebo API
+Co budeš u nás dělat:
+Vytvářet jednoduché automatizační nástroje pro kolegy
+Podílet se na složitějších řešeních, které budou používat celá oddělení
+Spolupracovat a hledat možnosti jak může AI a jiné technologie ulehčit naši práci
+Udržovat, opravovat a vylepšovat stávající řešení
+Používat ChatGPT, Copiloty a Git na denní bázi
+Časem ovládat spoustu daňových a účetních výrazů 😊
+def a_hodne():
+try:
+print(testovat)
+except NameError:
+print("testovat!")
+S čím budeš pracovat:
+Naše současné řešení jsou ve VBA, Power Automate a Pythonu
+Pro robotizace používáme RPA Power Automate Desktop
+Prostředí - Windows
+Hodně pracujeme s Excelovskými tabulkami, XML soubory, účetním systémem Helios a databázemi
+Co ti nabídneme:
+Flexibilní pracovní dobu
+Velmi zajímavé platové ohodnocení
+Mladý dynamický kolektiv příjemné pracovní prostředí v centru Prahy
+Profesní růst a odborné vzdělávání
+Zajímavé platové ohodnocení + pravidelné bonusy
+Zaměstnanecké benefity (dovolená navíc, stravenkový paušál, systém cafeterie - individuální čerpání benefitů, jazykové a odborné vzdělávání, pravidelné teambuildingy)
+Flexibilní pracovní dobu, možnost práce z domova
+Občerstvení na pracovišti každý den</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Petra Hořejší</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>224 931 366</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>&lt;div&gt;&lt;p&gt;Pracovní nabídka&lt;/p&gt;&lt;p&gt;&lt;strong&gt;ASB Group je profesionální outsourcingová společnost poskytující služby nadstandardní úrovně v oblasti zakládání společností, účetnictví, reportingu, daňového poradenství, trust managementu a mzdové agendy. Vznikla v roce 2002 a na pobočkách v Praze, Varšavě, Bratislavě, Budapešti a také Toruni zaměstnává přes 400 lidí. ASB Czech Republic s.r.o. právě rozšiřuje řady automatizačního týmu. Hledáme novou posilu s drivem a autentickým zájmem o automatizace, optimalizace, zlepšování procesů. Hledáme talentovaného nadšence, který se nebojí velkých výzev.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Baví tě hledat způsoby jak dělat věci efektivněji? Jsi schopný/á vést s nadšením konverzaci o technologiích od rána do večera? Změnila ti ChatGPT aspoň trochu život?&lt;/p&gt;&lt;p&gt;Nechceš si to v práci jen odsedět, ale investovat do toho něco sám/a za sebe? Už jsi někdy použil/a pozdrav „Hello, World!"? Hledáme juniorního kolegu do automatizačního týmu. Ve spolupráci s týmovým kolegou budeš mít stále dost velkou odpovědnost a tvoje rozhodnutí budou udávat dlouhodobý směr automatizace v naší firmě. Zároveň ale budeš mít vždy na koho se obrátit a kdo tě v případě potřeby povede.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Co budeme potřebovat:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Analytické myšlení a proaktivní přístup&lt;/li&gt;&lt;li&gt;Dobrou spolupráci jak remote, tak v kanceláři&lt;/li&gt;&lt;li&gt;SELECT * FROM zaklady_SQL;&lt;/li&gt;&lt;li&gt;Pokročilou znalost Excelu&lt;/li&gt;&lt;li&gt;Aktivní komunikaci v AJ alespoň na úrovni B1&lt;/li&gt;&lt;li&gt;Schopnost naučit se nové technologie (jazyk, platforma, ERP, AI nástroj)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Bude super, když budeš mít:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Mírně pokročilou znalost nějakého programovacího jazyka&lt;/li&gt;&lt;li&gt;Zkušenost s aktivním používáním AI&lt;/li&gt;&lt;li&gt;Jakékoliv zkušenosti s MS Power platformou, testováním aplikací, RPA nebo API&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Co budeš u nás dělat:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Vytvářet jednoduché automatizační nástroje pro kolegy&lt;/li&gt;&lt;li&gt;Podílet se na složitějších řešeních, které budou používat celá oddělení&lt;/li&gt;&lt;li&gt;Spolupracovat a hledat možnosti jak může AI a jiné technologie ulehčit naši práci&lt;/li&gt;&lt;li&gt;Udržovat, opravovat a vylepšovat stávající řešení&lt;/li&gt;&lt;li&gt;Používat ChatGPT, Copiloty a Git na denní bázi&lt;/li&gt;&lt;li&gt;Časem ovládat spoustu daňových a účetních výrazů 😊&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;em&gt;def a_hodne():&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; try:&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; print(testovat)&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; except NameError:&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; print("testovat!")&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;S čím budeš pracovat:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Naše současné řešení jsou ve VBA, Power Automate a Pythonu&lt;/li&gt;&lt;li&gt;Pro robotizace používáme RPA Power Automate Desktop&lt;/li&gt;&lt;li&gt;Prostředí - Windows&lt;/li&gt;&lt;li&gt;Hodně pracujeme s Excelovskými tabulkami, XML soubory, účetním systémem Helios a databázemi&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Co ti nabídneme:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Flexibilní pracovní dobu&lt;/li&gt;&lt;li&gt;Velmi zajímavé platové ohodnocení&lt;/li&gt;&lt;li&gt;Mladý dynamický kolektiv příjemné pracovní prostředí v centru Prahy&lt;/li&gt;&lt;li&gt;Profesní růst a odborné vzdělávání&lt;/li&gt;&lt;li&gt;Zajímavé platové ohodnocení + pravidelné bonusy&lt;/li&gt;&lt;li&gt;Zaměstnanecké benefity (dovolená navíc, stravenkový paušál, systém cafeterie - individuální čerpání benefitů, jazykové a odborné vzdělávání, pravidelné teambuildingy)&lt;/li&gt;&lt;li&gt;Flexibilní pracovní dobu, možnost práce z domova&lt;/li&gt;&lt;li&gt;Občerstvení na pracovišti každý den&lt;/li&gt;&lt;/ul&gt;&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Automation Developer</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ASB Czech Republic, s.r.o.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>V celnici 1031/4</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Praha</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Nové Město</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Pracovní nabídka
+ASB Group je profesionální outsourcingová společnost poskytující služby nadstandardní úrovně v oblasti zakládání společností, účetnictví, reportingu, daňového poradenství, trust managementu a mzdové agendy. Vznikla v roce 2002 a na pobočkách v Praze, Varšavě, Bratislavě, Budapešti a také Toruni zaměstnává přes 400 lidí. ASB Czech Republic s.r.o. právě rozšiřuje řady automatizačního týmu. Hledáme novou posilu s drivem a autentickým zájmem o automatizace, optimalizace, zlepšování procesů. Hledáme talentovaného nadšence, který se nebojí velkých výzev.
+Baví tě hledat způsoby jak dělat věci efektivněji? Jsi schopný/á vést s nadšením konverzaci o technologiích od rána do večera? Změnila ti ChatGPT aspoň trochu život?
+Nechceš si to v práci jen odsedět, ale investovat do toho něco sám/a za sebe? Už jsi někdy použil/a pozdrav „Hello, World!"? Hledáme juniorního kolegu do automatizačního týmu. Ve spolupráci s týmovým kolegou budeš mít stále dost velkou odpovědnost a tvoje rozhodnutí budou udávat dlouhodobý směr automatizace v naší firmě. Zároveň ale budeš mít vždy na koho se obrátit a kdo tě v případě potřeby povede.
+Co budeme potřebovat:
+Analytické myšlení a proaktivní přístup
+Dobrou spolupráci jak remote, tak v kanceláři
+SELECT * FROM zaklady_SQL;
+Pokročilou znalost Excelu
+Aktivní komunikaci v AJ alespoň na úrovni B1
+Schopnost naučit se nové technologie (jazyk, platforma, ERP, AI nástroj)
+Bude super, když budeš mít:
+Mírně pokročilou znalost nějakého programovacího jazyka
+Zkušenost s aktivním používáním AI
+Jakékoliv zkušenosti s MS Power platformou, testováním aplikací, RPA nebo API
+Co budeš u nás dělat:
+Vytvářet jednoduché automatizační nástroje pro kolegy
+Podílet se na složitějších řešeních, které budou používat celá oddělení
+Spolupracovat a hledat možnosti jak může AI a jiné technologie ulehčit naši práci
+Udržovat, opravovat a vylepšovat stávající řešení
+Používat ChatGPT, Copiloty a Git na denní bázi
+Časem ovládat spoustu daňových a účetních výrazů 😊
+def a_hodne():
+try:
+print(testovat)
+except NameError:
+print("testovat!")
+S čím budeš pracovat:
+Naše současné řešení jsou ve VBA, Power Automate a Pythonu
+Pro robotizace používáme RPA Power Automate Desktop
+Prostředí - Windows
+Hodně pracujeme s Excelovskými tabulkami, XML soubory, účetním systémem Helios a databázemi
+Co ti nabídneme:
+Flexibilní pracovní dobu
+Velmi zajímavé platové ohodnocení
+Mladý dynamický kolektiv příjemné pracovní prostředí v centru Prahy
+Profesní růst a odborné vzdělávání
+Zajímavé platové ohodnocení + pravidelné bonusy
+Zaměstnanecké benefity (dovolená navíc, stravenkový paušál, systém cafeterie - individuální čerpání benefitů, jazykové a odborné vzdělávání, pravidelné teambuildingy)
+Flexibilní pracovní dobu, možnost práce z domova
+Občerstvení na pracovišti každý den</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Petra Hořejší</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>224 931 366</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>&lt;div&gt;&lt;p&gt;Pracovní nabídka&lt;/p&gt;&lt;p&gt;&lt;strong&gt;ASB Group je profesionální outsourcingová společnost poskytující služby nadstandardní úrovně v oblasti zakládání společností, účetnictví, reportingu, daňového poradenství, trust managementu a mzdové agendy. Vznikla v roce 2002 a na pobočkách v Praze, Varšavě, Bratislavě, Budapešti a také Toruni zaměstnává přes 400 lidí. ASB Czech Republic s.r.o. právě rozšiřuje řady automatizačního týmu. Hledáme novou posilu s drivem a autentickým zájmem o automatizace, optimalizace, zlepšování procesů. Hledáme talentovaného nadšence, který se nebojí velkých výzev.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Baví tě hledat způsoby jak dělat věci efektivněji? Jsi schopný/á vést s nadšením konverzaci o technologiích od rána do večera? Změnila ti ChatGPT aspoň trochu život?&lt;/p&gt;&lt;p&gt;Nechceš si to v práci jen odsedět, ale investovat do toho něco sám/a za sebe? Už jsi někdy použil/a pozdrav „Hello, World!"? Hledáme juniorního kolegu do automatizačního týmu. Ve spolupráci s týmovým kolegou budeš mít stále dost velkou odpovědnost a tvoje rozhodnutí budou udávat dlouhodobý směr automatizace v naší firmě. Zároveň ale budeš mít vždy na koho se obrátit a kdo tě v případě potřeby povede.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Co budeme potřebovat:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Analytické myšlení a proaktivní přístup&lt;/li&gt;&lt;li&gt;Dobrou spolupráci jak remote, tak v kanceláři&lt;/li&gt;&lt;li&gt;SELECT * FROM zaklady_SQL;&lt;/li&gt;&lt;li&gt;Pokročilou znalost Excelu&lt;/li&gt;&lt;li&gt;Aktivní komunikaci v AJ alespoň na úrovni B1&lt;/li&gt;&lt;li&gt;Schopnost naučit se nové technologie (jazyk, platforma, ERP, AI nástroj)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Bude super, když budeš mít:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Mírně pokročilou znalost nějakého programovacího jazyka&lt;/li&gt;&lt;li&gt;Zkušenost s aktivním používáním AI&lt;/li&gt;&lt;li&gt;Jakékoliv zkušenosti s MS Power platformou, testováním aplikací, RPA nebo API&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Co budeš u nás dělat:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Vytvářet jednoduché automatizační nástroje pro kolegy&lt;/li&gt;&lt;li&gt;Podílet se na složitějších řešeních, které budou používat celá oddělení&lt;/li&gt;&lt;li&gt;Spolupracovat a hledat možnosti jak může AI a jiné technologie ulehčit naši práci&lt;/li&gt;&lt;li&gt;Udržovat, opravovat a vylepšovat stávající řešení&lt;/li&gt;&lt;li&gt;Používat ChatGPT, Copiloty a Git na denní bázi&lt;/li&gt;&lt;li&gt;Časem ovládat spoustu daňových a účetních výrazů 😊&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;em&gt;def a_hodne():&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; try:&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; print(testovat)&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; except NameError:&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; print("testovat!")&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;S čím budeš pracovat:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Naše současné řešení jsou ve VBA, Power Automate a Pythonu&lt;/li&gt;&lt;li&gt;Pro robotizace používáme RPA Power Automate Desktop&lt;/li&gt;&lt;li&gt;Prostředí - Windows&lt;/li&gt;&lt;li&gt;Hodně pracujeme s Excelovskými tabulkami, XML soubory, účetním systémem Helios a databázemi&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Co ti nabídneme:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Flexibilní pracovní dobu&lt;/li&gt;&lt;li&gt;Velmi zajímavé platové ohodnocení&lt;/li&gt;&lt;li&gt;Mladý dynamický kolektiv příjemné pracovní prostředí v centru Prahy&lt;/li&gt;&lt;li&gt;Profesní růst a odborné vzdělávání&lt;/li&gt;&lt;li&gt;Zajímavé platové ohodnocení + pravidelné bonusy&lt;/li&gt;&lt;li&gt;Zaměstnanecké benefity (dovolená navíc, stravenkový paušál, systém cafeterie - individuální čerpání benefitů, jazykové a odborné vzdělávání, pravidelné teambuildingy)&lt;/li&gt;&lt;li&gt;Flexibilní pracovní dobu, možnost práce z domova&lt;/li&gt;&lt;li&gt;Občerstvení na pracovišti každý den&lt;/li&gt;&lt;/ul&gt;&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Automation Developer</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ASB Czech Republic, s.r.o.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>V celnici 1031/4</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Praha</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Nové Město</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Pracovní nabídka
+ASB Group je profesionální outsourcingová společnost poskytující služby nadstandardní úrovně v oblasti zakládání společností, účetnictví, reportingu, daňového poradenství, trust managementu a mzdové agendy. Vznikla v roce 2002 a na pobočkách v Praze, Varšavě, Bratislavě, Budapešti a také Toruni zaměstnává přes 400 lidí. ASB Czech Republic s.r.o. právě rozšiřuje řady automatizačního týmu. Hledáme novou posilu s drivem a autentickým zájmem o automatizace, optimalizace, zlepšování procesů. Hledáme talentovaného nadšence, který se nebojí velkých výzev.
+Baví tě hledat způsoby jak dělat věci efektivněji? Jsi schopný/á vést s nadšením konverzaci o technologiích od rána do večera? Změnila ti ChatGPT aspoň trochu život?
+Nechceš si to v práci jen odsedět, ale investovat do toho něco sám/a za sebe? Už jsi někdy použil/a pozdrav „Hello, World!"? Hledáme juniorního kolegu do automatizačního týmu. Ve spolupráci s týmovým kolegou budeš mít stále dost velkou odpovědnost a tvoje rozhodnutí budou udávat dlouhodobý směr automatizace v naší firmě. Zároveň ale budeš mít vždy na koho se obrátit a kdo tě v případě potřeby povede.
+Co budeme potřebovat:
+Analytické myšlení a proaktivní přístup
+Dobrou spolupráci jak remote, tak v kanceláři
+SELECT * FROM zaklady_SQL;
+Pokročilou znalost Excelu
+Aktivní komunikaci v AJ alespoň na úrovni B1
+Schopnost naučit se nové technologie (jazyk, platforma, ERP, AI nástroj)
+Bude super, když budeš mít:
+Mírně pokročilou znalost nějakého programovacího jazyka
+Zkušenost s aktivním používáním AI
+Jakékoliv zkušenosti s MS Power platformou, testováním aplikací, RPA nebo API
+Co budeš u nás dělat:
+Vytvářet jednoduché automatizační nástroje pro kolegy
+Podílet se na složitějších řešeních, které budou používat celá oddělení
+Spolupracovat a hledat možnosti jak může AI a jiné technologie ulehčit naši práci
+Udržovat, opravovat a vylepšovat stávající řešení
+Používat ChatGPT, Copiloty a Git na denní bázi
+Časem ovládat spoustu daňových a účetních výrazů 😊
+def a_hodne():
+try:
+print(testovat)
+except NameError:
+print("testovat!")
+S čím budeš pracovat:
+Naše současné řešení jsou ve VBA, Power Automate a Pythonu
+Pro robotizace používáme RPA Power Automate Desktop
+Prostředí - Windows
+Hodně pracujeme s Excelovskými tabulkami, XML soubory, účetním systémem Helios a databázemi
+Co ti nabídneme:
+Flexibilní pracovní dobu
+Velmi zajímavé platové ohodnocení
+Mladý dynamický kolektiv příjemné pracovní prostředí v centru Prahy
+Profesní růst a odborné vzdělávání
+Zajímavé platové ohodnocení + pravidelné bonusy
+Zaměstnanecké benefity (dovolená navíc, stravenkový paušál, systém cafeterie - individuální čerpání benefitů, jazykové a odborné vzdělávání, pravidelné teambuildingy)
+Flexibilní pracovní dobu, možnost práce z domova
+Občerstvení na pracovišti každý den</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Petra Hořejší</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>224 931 366</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>&lt;div&gt;&lt;p&gt;Pracovní nabídka&lt;/p&gt;&lt;p&gt;&lt;strong&gt;ASB Group je profesionální outsourcingová společnost poskytující služby nadstandardní úrovně v oblasti zakládání společností, účetnictví, reportingu, daňového poradenství, trust managementu a mzdové agendy. Vznikla v roce 2002 a na pobočkách v Praze, Varšavě, Bratislavě, Budapešti a také Toruni zaměstnává přes 400 lidí. ASB Czech Republic s.r.o. právě rozšiřuje řady automatizačního týmu. Hledáme novou posilu s drivem a autentickým zájmem o automatizace, optimalizace, zlepšování procesů. Hledáme talentovaného nadšence, který se nebojí velkých výzev.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Baví tě hledat způsoby jak dělat věci efektivněji? Jsi schopný/á vést s nadšením konverzaci o technologiích od rána do večera? Změnila ti ChatGPT aspoň trochu život?&lt;/p&gt;&lt;p&gt;Nechceš si to v práci jen odsedět, ale investovat do toho něco sám/a za sebe? Už jsi někdy použil/a pozdrav „Hello, World!"? Hledáme juniorního kolegu do automatizačního týmu. Ve spolupráci s týmovým kolegou budeš mít stále dost velkou odpovědnost a tvoje rozhodnutí budou udávat dlouhodobý směr automatizace v naší firmě. Zároveň ale budeš mít vždy na koho se obrátit a kdo tě v případě potřeby povede.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Co budeme potřebovat:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Analytické myšlení a proaktivní přístup&lt;/li&gt;&lt;li&gt;Dobrou spolupráci jak remote, tak v kanceláři&lt;/li&gt;&lt;li&gt;SELECT * FROM zaklady_SQL;&lt;/li&gt;&lt;li&gt;Pokročilou znalost Excelu&lt;/li&gt;&lt;li&gt;Aktivní komunikaci v AJ alespoň na úrovni B1&lt;/li&gt;&lt;li&gt;Schopnost naučit se nové technologie (jazyk, platforma, ERP, AI nástroj)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Bude super, když budeš mít:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Mírně pokročilou znalost nějakého programovacího jazyka&lt;/li&gt;&lt;li&gt;Zkušenost s aktivním používáním AI&lt;/li&gt;&lt;li&gt;Jakékoliv zkušenosti s MS Power platformou, testováním aplikací, RPA nebo API&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Co budeš u nás dělat:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Vytvářet jednoduché automatizační nástroje pro kolegy&lt;/li&gt;&lt;li&gt;Podílet se na složitějších řešeních, které budou používat celá oddělení&lt;/li&gt;&lt;li&gt;Spolupracovat a hledat možnosti jak může AI a jiné technologie ulehčit naši práci&lt;/li&gt;&lt;li&gt;Udržovat, opravovat a vylepšovat stávající řešení&lt;/li&gt;&lt;li&gt;Používat ChatGPT, Copiloty a Git na denní bázi&lt;/li&gt;&lt;li&gt;Časem ovládat spoustu daňových a účetních výrazů 😊&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;em&gt;def a_hodne():&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; try:&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; print(testovat)&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; except NameError:&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; print("testovat!")&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;S čím budeš pracovat:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Naše současné řešení jsou ve VBA, Power Automate a Pythonu&lt;/li&gt;&lt;li&gt;Pro robotizace používáme RPA Power Automate Desktop&lt;/li&gt;&lt;li&gt;Prostředí - Windows&lt;/li&gt;&lt;li&gt;Hodně pracujeme s Excelovskými tabulkami, XML soubory, účetním systémem Helios a databázemi&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Co ti nabídneme:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Flexibilní pracovní dobu&lt;/li&gt;&lt;li&gt;Velmi zajímavé platové ohodnocení&lt;/li&gt;&lt;li&gt;Mladý dynamický kolektiv příjemné pracovní prostředí v centru Prahy&lt;/li&gt;&lt;li&gt;Profesní růst a odborné vzdělávání&lt;/li&gt;&lt;li&gt;Zajímavé platové ohodnocení + pravidelné bonusy&lt;/li&gt;&lt;li&gt;Zaměstnanecké benefity (dovolená navíc, stravenkový paušál, systém cafeterie - individuální čerpání benefitů, jazykové a odborné vzdělávání, pravidelné teambuildingy)&lt;/li&gt;&lt;li&gt;Flexibilní pracovní dobu, možnost práce z domova&lt;/li&gt;&lt;li&gt;Občerstvení na pracovišti každý den&lt;/li&gt;&lt;/ul&gt;&lt;/div&gt;</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updates in something i forgot
</commit_message>
<xml_diff>
--- a/jobs_data.xlsx
+++ b/jobs_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1198,7 +1198,94 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Vývojář/Analytik Databáze/SQL</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>SEACOMP s.r.o.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Brandlova 253/4</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Brno</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Brno-město</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Pracovní nabídka
+Staňte se součástí logistické divize SEACOMP vyvíjející rozsáhlé robotizované logistické informační systémy. Podílíme se na implementaci a managementu produkčních systémů o velikosti až 120.000 m2 v rámci celého evropského prostoru.
+Předmětem Vaší práce bude:
+- Vývoj backendu logistického informačního systému – platforma PL/SQL
+- Návrh a implementace změn ve warehouse procesech s důrazem na zvyšování výkonnosti
+- Nasazení implementace do produkčního systému
+- Provádění integračních a akceptačních testů
+Požadujeme:
+- Práce na plný úvazek, přechodně možno i na částečný
+- Znalost programování relačních databází (ORACLE není podmínkou): SQL nebo některý ze strukturovaných jazyků (I-SQL, T-SQL, PL/SQL, …)
+- Aktivní přístup při řešení projektů
+- Vysokoškolské vzdělání technického směru
+- Zodpovědnost a smysl pro práci v týmu
+Nabízíme:
+- Nadstandardní platové ohodnocení – nechte si vypracovat individuální nabídku, talenty umíme ocenit
+- Pružná pracovní doba – máme řešení pro ranní ptáčata i večerní sovy
+- Přátelské a kolegiální pracovní prostředí ve zcela nové polyfunkční budově v naprostém centru Brna
+- Odborné školení, možnost seznámit se s širokým spektrem aktuálních vývojových technologií
+- Možnost krátkodobých služebních cest do zahraničí
+- Možnost využít firemní chill-out zónu přímo na pracovišti (fotbálek, ergonometr, rotoped, grill bar, aj.)
+- Penzijní připojištění, příspěvky na stravování, mobilní telefon, notebook
+- Široká škála mimofiremních aktivit (dračí lodě, cyklovýlety, lyžování, sportovní turnaje, …)
+Nástup je možný ihned nebo dle dohody.
+Pokud máte o tuto pozici zájem, pošlete prosím Váš strukturovaný životopis na e-mail jobs(a)seacomp.cz nebo nás kontaktuje telefonicky na tel. čísle + 420 608 736 650
+Velmi se těšíme se na spolupráci s Vámi.
+SEACOMP S.R.O., BRANDLOVA 4, 602 00 BRNO, DRŽITEL CERTIFIKACE ISO 9001:2015 ISO 14001:2015 ISO 27001:2013</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>David Bryša</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>539 030 661</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>['PL/SQL', 'SQL', 'ORACLE', 'I-SQL', 'warehouse', 'T-SQL']</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>&lt;div&gt;&lt;p&gt;Pracovní nabídka&lt;/p&gt;&lt;p&gt;Staňte se součástí logistické divize SEACOMP vyvíjející rozsáhlé robotizované logistické informační systémy. Podílíme se na implementaci a managementu produkčních systémů o velikosti až 120.000 m2 v rámci celého evropského prostoru. &lt;br&gt; &lt;br&gt;Předmětem Vaší práce bude: &lt;br&gt; &lt;br&gt;- Vývoj backendu logistického informačního systému – platforma PL/SQL &lt;br&gt;&lt;/br&gt;- Návrh a implementace změn ve warehouse procesech s důrazem na zvyšování výkonnosti&lt;br&gt;&lt;/br&gt;- Nasazení implementace do produkčního systému &lt;br&gt;&lt;/br&gt; - Provádění integračních a akceptačních testů&lt;br&gt;&lt;/br&gt;&lt;br&gt;&lt;/br&gt;Požadujeme: &lt;br&gt;&lt;/br&gt; &lt;br&gt;&lt;/br&gt;- Práce na plný úvazek, přechodně možno i na částečný &lt;br&gt;&lt;/br&gt;- Znalost programování relačních databází (ORACLE není podmínkou): SQL nebo některý ze strukturovaných jazyků (I-SQL, T-SQL, PL/SQL, …) &lt;br&gt;&lt;/br&gt;- Aktivní přístup při řešení projektů &lt;br&gt;&lt;/br&gt;- Vysokoškolské vzdělání technického směru &lt;br&gt;&lt;/br&gt;- Zodpovědnost a smysl pro práci v týmu &lt;br&gt;&lt;/br&gt; &lt;br&gt;&lt;/br&gt;Nabízíme:&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;&lt;/p&gt;&lt;p&gt;- Nadstandardní platové ohodnocení – nechte si vypracovat individuální nabídku, talenty umíme ocenit&lt;br&gt;&lt;/br&gt;- Pružná pracovní doba – máme řešení pro ranní ptáčata i večerní sovy&lt;br&gt;&lt;/br&gt;- Přátelské a kolegiální pracovní prostředí ve zcela nové polyfunkční budově v naprostém centru Brna&lt;br&gt;&lt;/br&gt;- Odborné školení, možnost seznámit se s širokým spektrem aktuálních vývojových technologií&lt;br&gt;&lt;/br&gt;- Možnost krátkodobých služebních cest do zahraničí&lt;br&gt;&lt;/br&gt;- Možnost využít firemní chill-out zónu přímo na pracovišti (fotbálek, ergonometr, rotoped, grill bar, aj.)&lt;br&gt;&lt;/br&gt;- Penzijní připojištění, příspěvky na stravování, mobilní telefon, notebook&lt;br&gt;&lt;/br&gt;- Široká škála mimofiremních aktivit (dračí lodě, cyklovýlety, lyžování, sportovní turnaje, …)&lt;/p&gt;&lt;p&gt;Nástup je možný ihned nebo dle dohody.&lt;/p&gt;&lt;p&gt;Pokud máte o tuto pozici zájem, pošlete prosím Váš strukturovaný životopis na e-mail jobs(a)seacomp.cz nebo nás kontaktuje telefonicky na tel. čísle + 420 608 736 650&lt;/p&gt;&lt;p&gt;Velmi se těšíme se na spolupráci s Vámi.&lt;/p&gt;&lt;p&gt;SEACOMP S.R.O., BRANDLOVA 4, 602 00 BRNO, DRŽITEL CERTIFIKACE ISO 9001:2015 ISO 14001:2015 ISO 27001:2013&lt;/p&gt;&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{6e0a5f83-1728-4956-bdf4-ce37760cd214}" enabled="0" method="" siteId="{6e0a5f83-1728-4956-bdf4-ce37760cd214}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>